<commit_message>
feature importance is done
</commit_message>
<xml_diff>
--- a/all-results-trimed.xlsx
+++ b/all-results-trimed.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumensardar/Documents/Projects/scm4.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0807FFD6-1BDE-5A40-9C8F-BDC9BD441A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63865ACC-E581-A742-A92F-9FFBD75592DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all-results" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
     <sheet name="baseline" sheetId="2" r:id="rId3"/>
     <sheet name="dataset" sheetId="3" r:id="rId4"/>
+    <sheet name="feature-importance" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'all-results'!$A$1:$T$41</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="146">
   <si>
     <t>Duration</t>
   </si>
@@ -405,13 +406,88 @@
   </si>
   <si>
     <t>2nd Best</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>item_id&amp;day_of_week</t>
+  </si>
+  <si>
+    <t>day_of_week</t>
+  </si>
+  <si>
+    <t>shop_id</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>GEOGRAPHY_DESC&amp;UNIT_DESC</t>
+  </si>
+  <si>
+    <t>GEOGRAPHY_DESC</t>
+  </si>
+  <si>
+    <t>UNIT_DESC</t>
+  </si>
+  <si>
+    <t>HS_CODE</t>
+  </si>
+  <si>
+    <t>GEOGRAPHY_CODE</t>
+  </si>
+  <si>
+    <t>CustomerID&amp;Country</t>
+  </si>
+  <si>
+    <t>Country&amp;day</t>
+  </si>
+  <si>
+    <t>StockCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>Price&amp;month</t>
+  </si>
+  <si>
+    <t>Price&amp;day</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Warehouse&amp;month</t>
+  </si>
+  <si>
+    <t>Top Feature Rank#1</t>
+  </si>
+  <si>
+    <t>Top Feature Rank#2</t>
+  </si>
+  <si>
+    <t>Top Feature Rank#3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,6 +676,13 @@
       <i/>
       <u/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -1016,7 +1099,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1059,12 +1142,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1072,9 +1149,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1088,6 +1162,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1549,7 +1642,7 @@
         <v>53</v>
       </c>
       <c r="G2">
-        <f>H2+L2</f>
+        <f t="shared" ref="G2:G41" si="0">H2+L2</f>
         <v>2935849</v>
       </c>
       <c r="H2">
@@ -1612,7 +1705,7 @@
         <v>25</v>
       </c>
       <c r="G3">
-        <f>H3+L3</f>
+        <f t="shared" si="0"/>
         <v>2935849</v>
       </c>
       <c r="H3">
@@ -1675,7 +1768,7 @@
         <v>20</v>
       </c>
       <c r="G4">
-        <f>H4+L4</f>
+        <f t="shared" si="0"/>
         <v>2935849</v>
       </c>
       <c r="H4">
@@ -1738,7 +1831,7 @@
         <v>55</v>
       </c>
       <c r="G5">
-        <f>H5+L5</f>
+        <f t="shared" si="0"/>
         <v>2935849</v>
       </c>
       <c r="H5">
@@ -1801,7 +1894,7 @@
         <v>53</v>
       </c>
       <c r="G6">
-        <f>H6+L6</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H6">
@@ -1864,7 +1957,7 @@
         <v>25</v>
       </c>
       <c r="G7">
-        <f>H7+L7</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H7">
@@ -1927,7 +2020,7 @@
         <v>20</v>
       </c>
       <c r="G8">
-        <f>H8+L8</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H8">
@@ -1990,7 +2083,7 @@
         <v>55</v>
       </c>
       <c r="G9">
-        <f>H9+L9</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H9">
@@ -2053,7 +2146,7 @@
         <v>53</v>
       </c>
       <c r="G10">
-        <f>H10+L10</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H10">
@@ -2116,7 +2209,7 @@
         <v>25</v>
       </c>
       <c r="G11">
-        <f>H11+L11</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H11">
@@ -2179,7 +2272,7 @@
         <v>20</v>
       </c>
       <c r="G12">
-        <f>H12+L12</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H12">
@@ -2242,7 +2335,7 @@
         <v>55</v>
       </c>
       <c r="G13">
-        <f>H13+L13</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H13">
@@ -2305,7 +2398,7 @@
         <v>53</v>
       </c>
       <c r="G14">
-        <f>H14+L14</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H14">
@@ -2368,7 +2461,7 @@
         <v>25</v>
       </c>
       <c r="G15">
-        <f>H15+L15</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H15">
@@ -2431,7 +2524,7 @@
         <v>20</v>
       </c>
       <c r="G16">
-        <f>H16+L16</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H16">
@@ -2494,7 +2587,7 @@
         <v>55</v>
       </c>
       <c r="G17">
-        <f>H17+L17</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H17">
@@ -2557,7 +2650,7 @@
         <v>53</v>
       </c>
       <c r="G18">
-        <f>H18+L18</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H18">
@@ -2620,7 +2713,7 @@
         <v>25</v>
       </c>
       <c r="G19">
-        <f>H19+L19</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H19">
@@ -2683,7 +2776,7 @@
         <v>20</v>
       </c>
       <c r="G20">
-        <f>H20+L20</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H20">
@@ -2746,7 +2839,7 @@
         <v>55</v>
       </c>
       <c r="G21">
-        <f>H21+L21</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H21">
@@ -2809,7 +2902,7 @@
         <v>53</v>
       </c>
       <c r="G22">
-        <f>H22+L22</f>
+        <f t="shared" si="0"/>
         <v>2935849</v>
       </c>
       <c r="H22">
@@ -2872,7 +2965,7 @@
         <v>25</v>
       </c>
       <c r="G23">
-        <f>H23+L23</f>
+        <f t="shared" si="0"/>
         <v>2935849</v>
       </c>
       <c r="H23">
@@ -2935,7 +3028,7 @@
         <v>20</v>
       </c>
       <c r="G24">
-        <f>H24+L24</f>
+        <f t="shared" si="0"/>
         <v>2935849</v>
       </c>
       <c r="H24">
@@ -2998,7 +3091,7 @@
         <v>55</v>
       </c>
       <c r="G25">
-        <f>H25+L25</f>
+        <f t="shared" si="0"/>
         <v>2935849</v>
       </c>
       <c r="H25">
@@ -3061,7 +3154,7 @@
         <v>53</v>
       </c>
       <c r="G26">
-        <f>H26+L26</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H26">
@@ -3124,7 +3217,7 @@
         <v>25</v>
       </c>
       <c r="G27">
-        <f>H27+L27</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H27">
@@ -3187,7 +3280,7 @@
         <v>20</v>
       </c>
       <c r="G28">
-        <f>H28+L28</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H28">
@@ -3250,7 +3343,7 @@
         <v>55</v>
       </c>
       <c r="G29">
-        <f>H29+L29</f>
+        <f t="shared" si="0"/>
         <v>237165</v>
       </c>
       <c r="H29">
@@ -3313,7 +3406,7 @@
         <v>53</v>
       </c>
       <c r="G30">
-        <f>H30+L30</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H30">
@@ -3376,7 +3469,7 @@
         <v>25</v>
       </c>
       <c r="G31">
-        <f>H31+L31</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H31">
@@ -3439,7 +3532,7 @@
         <v>20</v>
       </c>
       <c r="G32">
-        <f>H32+L32</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H32">
@@ -3502,7 +3595,7 @@
         <v>55</v>
       </c>
       <c r="G33">
-        <f>H33+L33</f>
+        <f t="shared" si="0"/>
         <v>406829</v>
       </c>
       <c r="H33">
@@ -3565,7 +3658,7 @@
         <v>53</v>
       </c>
       <c r="G34">
-        <f>H34+L34</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H34">
@@ -3628,7 +3721,7 @@
         <v>25</v>
       </c>
       <c r="G35">
-        <f>H35+L35</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H35">
@@ -3691,7 +3784,7 @@
         <v>20</v>
       </c>
       <c r="G36">
-        <f>H36+L36</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H36">
@@ -3754,7 +3847,7 @@
         <v>55</v>
       </c>
       <c r="G37">
-        <f>H37+L37</f>
+        <f t="shared" si="0"/>
         <v>824364</v>
       </c>
       <c r="H37">
@@ -3817,7 +3910,7 @@
         <v>53</v>
       </c>
       <c r="G38">
-        <f>H38+L38</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H38">
@@ -3880,7 +3973,7 @@
         <v>25</v>
       </c>
       <c r="G39">
-        <f>H39+L39</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H39">
@@ -3943,7 +4036,7 @@
         <v>20</v>
       </c>
       <c r="G40">
-        <f>H40+L40</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H40">
@@ -4006,7 +4099,7 @@
         <v>55</v>
       </c>
       <c r="G41">
-        <f>H41+L41</f>
+        <f t="shared" si="0"/>
         <v>1037336</v>
       </c>
       <c r="H41">
@@ -6944,7 +7037,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
@@ -6952,44 +7045,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="16" t="b">
+      <c r="B3" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -7009,8 +7102,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="13" t="s">
         <v>118</v>
       </c>
@@ -7028,8 +7121,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="13" t="s">
         <v>117</v>
       </c>
@@ -7047,8 +7140,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="13" t="s">
         <v>116</v>
       </c>
@@ -7066,8 +7159,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="16" t="b">
+      <c r="A7" s="25"/>
+      <c r="B7" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -7087,8 +7180,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="13" t="s">
         <v>118</v>
       </c>
@@ -7106,8 +7199,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="13" t="s">
         <v>117</v>
       </c>
@@ -7125,8 +7218,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="13" t="s">
         <v>116</v>
       </c>
@@ -7144,10 +7237,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="16" t="b">
+      <c r="B11" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -7167,8 +7260,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="13" t="s">
         <v>118</v>
       </c>
@@ -7186,8 +7279,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="13" t="s">
         <v>117</v>
       </c>
@@ -7205,8 +7298,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="13" t="s">
         <v>116</v>
       </c>
@@ -7224,8 +7317,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="16" t="b">
+      <c r="A15" s="25"/>
+      <c r="B15" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -7245,8 +7338,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="13" t="s">
         <v>118</v>
       </c>
@@ -7264,8 +7357,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="13" t="s">
         <v>117</v>
       </c>
@@ -7283,8 +7376,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="13" t="s">
         <v>116</v>
       </c>
@@ -7302,10 +7395,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="16" t="b">
+      <c r="B19" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -7325,8 +7418,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="13" t="s">
         <v>118</v>
       </c>
@@ -7344,8 +7437,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="13" t="s">
         <v>117</v>
       </c>
@@ -7363,8 +7456,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="13" t="s">
         <v>116</v>
       </c>
@@ -7382,8 +7475,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="16" t="b">
+      <c r="A23" s="25"/>
+      <c r="B23" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -7403,8 +7496,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="16"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="13" t="s">
         <v>118</v>
       </c>
@@ -7422,8 +7515,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="13" t="s">
         <v>117</v>
       </c>
@@ -7441,8 +7534,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="16"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="13" t="s">
         <v>116</v>
       </c>
@@ -7460,10 +7553,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="16" t="b">
+      <c r="B27" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -7483,8 +7576,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="13" t="s">
         <v>118</v>
       </c>
@@ -7502,8 +7595,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="13" t="s">
         <v>117</v>
       </c>
@@ -7521,8 +7614,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="13" t="s">
         <v>116</v>
       </c>
@@ -7540,8 +7633,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
-      <c r="B31" s="16" t="b">
+      <c r="A31" s="25"/>
+      <c r="B31" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -7561,8 +7654,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="16"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="13" t="s">
         <v>118</v>
       </c>
@@ -7580,8 +7673,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="16"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="13" t="s">
         <v>117</v>
       </c>
@@ -7599,8 +7692,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="13" t="s">
         <v>116</v>
       </c>
@@ -7618,10 +7711,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="16" t="b">
+      <c r="B35" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C35" s="13" t="s">
@@ -7641,8 +7734,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="16"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="13" t="s">
         <v>118</v>
       </c>
@@ -7660,8 +7753,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="16"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="13" t="s">
         <v>117</v>
       </c>
@@ -7679,8 +7772,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="16"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="13" t="s">
         <v>116</v>
       </c>
@@ -7698,8 +7791,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="16" t="b">
+      <c r="A39" s="25"/>
+      <c r="B39" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C39" s="13" t="s">
@@ -7719,8 +7812,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="13" t="s">
         <v>118</v>
       </c>
@@ -7738,8 +7831,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="16"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="13" t="s">
         <v>117</v>
       </c>
@@ -7757,8 +7850,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="13" t="s">
         <v>116</v>
       </c>
@@ -7776,21 +7869,21 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="16" t="b">
+      <c r="B44" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C44" s="13" t="s">
@@ -7810,8 +7903,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="16"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="13" t="s">
         <v>118</v>
       </c>
@@ -7829,8 +7922,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="13" t="s">
         <v>117</v>
       </c>
@@ -7848,8 +7941,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="16"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="13" t="s">
         <v>116</v>
       </c>
@@ -7867,8 +7960,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="16" t="b">
+      <c r="A48" s="25"/>
+      <c r="B48" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="13" t="s">
@@ -7888,8 +7981,8 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="16"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="13" t="s">
         <v>118</v>
       </c>
@@ -7907,8 +8000,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="16"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="13" t="s">
         <v>117</v>
       </c>
@@ -7926,8 +8019,8 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="13" t="s">
         <v>116</v>
       </c>
@@ -7945,10 +8038,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A52" s="18" t="s">
+      <c r="A52" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="16" t="b">
+      <c r="B52" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C52" s="13" t="s">
@@ -7968,8 +8061,8 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="13" t="s">
         <v>118</v>
       </c>
@@ -7987,8 +8080,8 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="16"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="13" t="s">
         <v>117</v>
       </c>
@@ -8006,8 +8099,8 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
-      <c r="B55" s="16"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="24"/>
       <c r="C55" s="13" t="s">
         <v>116</v>
       </c>
@@ -8025,8 +8118,8 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="16" t="b">
+      <c r="A56" s="25"/>
+      <c r="B56" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C56" s="13" t="s">
@@ -8046,8 +8139,8 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="16"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="13" t="s">
         <v>118</v>
       </c>
@@ -8065,8 +8158,8 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
-      <c r="B58" s="16"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="24"/>
       <c r="C58" s="13" t="s">
         <v>117</v>
       </c>
@@ -8084,8 +8177,8 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="16"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="13" t="s">
         <v>116</v>
       </c>
@@ -8103,10 +8196,10 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B60" s="16" t="b">
+      <c r="B60" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C60" s="13" t="s">
@@ -8126,8 +8219,8 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="16"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="13" t="s">
         <v>118</v>
       </c>
@@ -8145,8 +8238,8 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="16"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="24"/>
       <c r="C62" s="13" t="s">
         <v>117</v>
       </c>
@@ -8164,8 +8257,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A63" s="18"/>
-      <c r="B63" s="16"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="13" t="s">
         <v>116</v>
       </c>
@@ -8183,8 +8276,8 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
-      <c r="B64" s="16" t="b">
+      <c r="A64" s="25"/>
+      <c r="B64" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C64" s="13" t="s">
@@ -8204,8 +8297,8 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A65" s="18"/>
-      <c r="B65" s="16"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="24"/>
       <c r="C65" s="13" t="s">
         <v>118</v>
       </c>
@@ -8223,8 +8316,8 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
-      <c r="B66" s="16"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="24"/>
       <c r="C66" s="13" t="s">
         <v>117</v>
       </c>
@@ -8242,8 +8335,8 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
-      <c r="B67" s="16"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="24"/>
       <c r="C67" s="13" t="s">
         <v>116</v>
       </c>
@@ -8261,10 +8354,10 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A68" s="18" t="s">
+      <c r="A68" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B68" s="16" t="b">
+      <c r="B68" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C68" s="13" t="s">
@@ -8284,8 +8377,8 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
-      <c r="B69" s="16"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="24"/>
       <c r="C69" s="13" t="s">
         <v>118</v>
       </c>
@@ -8303,8 +8396,8 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A70" s="18"/>
-      <c r="B70" s="16"/>
+      <c r="A70" s="25"/>
+      <c r="B70" s="24"/>
       <c r="C70" s="13" t="s">
         <v>117</v>
       </c>
@@ -8322,8 +8415,8 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A71" s="18"/>
-      <c r="B71" s="16"/>
+      <c r="A71" s="25"/>
+      <c r="B71" s="24"/>
       <c r="C71" s="13" t="s">
         <v>116</v>
       </c>
@@ -8341,8 +8434,8 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
-      <c r="B72" s="16" t="b">
+      <c r="A72" s="25"/>
+      <c r="B72" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C72" s="13" t="s">
@@ -8362,8 +8455,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
-      <c r="B73" s="16"/>
+      <c r="A73" s="25"/>
+      <c r="B73" s="24"/>
       <c r="C73" s="13" t="s">
         <v>118</v>
       </c>
@@ -8381,8 +8474,8 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A74" s="18"/>
-      <c r="B74" s="16"/>
+      <c r="A74" s="25"/>
+      <c r="B74" s="24"/>
       <c r="C74" s="13" t="s">
         <v>117</v>
       </c>
@@ -8400,8 +8493,8 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
-      <c r="B75" s="16"/>
+      <c r="A75" s="25"/>
+      <c r="B75" s="24"/>
       <c r="C75" s="13" t="s">
         <v>116</v>
       </c>
@@ -8419,10 +8512,10 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A76" s="18" t="s">
+      <c r="A76" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B76" s="16" t="b">
+      <c r="B76" s="24" t="b">
         <v>0</v>
       </c>
       <c r="C76" s="13" t="s">
@@ -8442,8 +8535,8 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
-      <c r="B77" s="16"/>
+      <c r="A77" s="25"/>
+      <c r="B77" s="24"/>
       <c r="C77" s="13" t="s">
         <v>118</v>
       </c>
@@ -8461,8 +8554,8 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
-      <c r="B78" s="16"/>
+      <c r="A78" s="25"/>
+      <c r="B78" s="24"/>
       <c r="C78" s="13" t="s">
         <v>117</v>
       </c>
@@ -8480,8 +8573,8 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
-      <c r="B79" s="16"/>
+      <c r="A79" s="25"/>
+      <c r="B79" s="24"/>
       <c r="C79" s="13" t="s">
         <v>116</v>
       </c>
@@ -8499,8 +8592,8 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
-      <c r="B80" s="16" t="b">
+      <c r="A80" s="25"/>
+      <c r="B80" s="24" t="b">
         <v>1</v>
       </c>
       <c r="C80" s="13" t="s">
@@ -8520,8 +8613,8 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A81" s="18"/>
-      <c r="B81" s="16"/>
+      <c r="A81" s="25"/>
+      <c r="B81" s="24"/>
       <c r="C81" s="13" t="s">
         <v>118</v>
       </c>
@@ -8539,8 +8632,8 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A82" s="18"/>
-      <c r="B82" s="16"/>
+      <c r="A82" s="25"/>
+      <c r="B82" s="24"/>
       <c r="C82" s="13" t="s">
         <v>117</v>
       </c>
@@ -8558,8 +8651,8 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A83" s="18"/>
-      <c r="B83" s="16"/>
+      <c r="A83" s="25"/>
+      <c r="B83" s="24"/>
       <c r="C83" s="13" t="s">
         <v>116</v>
       </c>
@@ -8578,22 +8671,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B35:B38"/>
     <mergeCell ref="A52:A59"/>
     <mergeCell ref="A60:A67"/>
     <mergeCell ref="A68:A75"/>
@@ -8610,6 +8687,22 @@
     <mergeCell ref="A27:A34"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A44:A51"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B35:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8619,7 +8712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556D1724-AF38-DB4D-B112-F6FEB531872D}">
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" workbookViewId="0">
+    <sheetView zoomScale="220" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -8634,31 +8727,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="21" t="b">
+      <c r="C2" s="26" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -8667,7 +8760,7 @@
       <c r="E2" s="12">
         <v>317530.90000000002</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>0.75</v>
       </c>
       <c r="G2" s="12">
@@ -8679,15 +8772,15 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="14" t="s">
         <v>81</v>
       </c>
       <c r="E3" s="12">
         <v>3375479.27</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="22">
         <v>0.65</v>
       </c>
       <c r="G3" s="12">
@@ -8699,10 +8792,10 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="13" t="s">
         <v>115</v>
       </c>
@@ -8720,8 +8813,8 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="28" x14ac:dyDescent="0.2">
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="13" t="s">
         <v>118</v>
       </c>
@@ -8739,8 +8832,8 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="13" t="s">
         <v>117</v>
       </c>
@@ -8758,8 +8851,8 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="13" t="s">
         <v>116</v>
       </c>
@@ -8777,14 +8870,14 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="21"/>
-      <c r="C8" s="16" t="b">
+      <c r="B8" s="26"/>
+      <c r="C8" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>687.66456746133804</v>
       </c>
       <c r="F8" s="13">
@@ -8798,8 +8891,8 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="28" x14ac:dyDescent="0.2">
-      <c r="B9" s="21"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="13" t="s">
         <v>118</v>
       </c>
@@ -8809,16 +8902,16 @@
       <c r="F9" s="13">
         <v>9.7377960620463504E+16</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="16">
         <v>38450217.344450898</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="16">
         <v>6200.8239246450903</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="21"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="13" t="s">
         <v>117</v>
       </c>
@@ -8828,20 +8921,20 @@
       <c r="F10" s="13">
         <v>2.5229963061592602E+17</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <v>105859045.184744</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <v>10288.782492828999</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="21"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="21">
         <v>1035.73425472177</v>
       </c>
       <c r="F11" s="13">
@@ -8855,39 +8948,39 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="26">
+      <c r="D14" s="18"/>
+      <c r="E14" s="23">
         <f>E2-E8</f>
         <v>316843.23543253867</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="26">
+      <c r="F14" s="18"/>
+      <c r="G14" s="23">
         <f>G2-G9</f>
         <v>167198928686.74445</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="23">
         <f>H2-H9</f>
         <v>402745.8460753549</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="26">
+      <c r="D15" s="18"/>
+      <c r="E15" s="23">
         <f>E2-E11</f>
         <v>316495.16574527824</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="26">
+      <c r="F15" s="18"/>
+      <c r="G15" s="23">
         <f>G2-G10</f>
         <v>167131519858.90414</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="23">
         <f>H2-H10</f>
         <v>398657.88750717096</v>
       </c>
@@ -8907,7 +9000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5943C64C-7BAE-554E-ABE2-93E3B1F0F6CB}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9402,4 +9495,382 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76786F9-7308-384A-8FB4-63DFA6842D5F}">
+  <dimension ref="C4:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C5" s="27"/>
+      <c r="D5" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C6" s="27"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C7" s="27"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C8" s="27"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="27"/>
+      <c r="D9" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="27"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="27"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="27"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="27"/>
+      <c r="D13" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C14" s="27"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="27"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C16" s="27"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="27"/>
+      <c r="D17" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="27"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="27"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="27"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="27"/>
+      <c r="D21" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="27"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="27"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="27"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D21:D24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>